<commit_message>
New changes in CheckOtherDeductions
</commit_message>
<xml_diff>
--- a/Documentation/TaxSolver Instance List.xlsx
+++ b/Documentation/TaxSolver Instance List.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\james.wilkinson\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://taxwarellc-my.sharepoint.com/personal/nahuel_delacruz_sovos_com/Documents/Desktop/Nahuel/Projects/STS Internal Review bot/Documentation/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B63D68B8-0B31-411A-9166-012C2D2F0C11}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="2" documentId="13_ncr:1_{B63D68B8-0B31-411A-9166-012C2D2F0C11}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{59EAE2B0-C386-4EB7-9C3D-D0D6A3E1B47E}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{44AAB872-1E4E-4FF4-9C89-3E765CB0CED9}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{44AAB872-1E4E-4FF4-9C89-3E765CB0CED9}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -2261,8 +2261,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{21B5D9E0-5F12-4839-AFE3-082EC7C5A69A}">
   <dimension ref="A1:D246"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A213" workbookViewId="0">
-      <selection activeCell="B232" sqref="B232"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C108" sqref="C108"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>